<commit_message>
First Table is Created By using UI
</commit_message>
<xml_diff>
--- a/SqlLessons.xlsx
+++ b/SqlLessons.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hasan\Desktop\MSSql\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4ADA2D43-7DCE-4B70-8972-BA679BC6B98D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF6C0EED-A329-4537-8C1D-F764F7978430}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="37">
   <si>
     <t>cutomer</t>
   </si>
@@ -133,6 +133,9 @@
   </si>
   <si>
     <t>char(3)</t>
+  </si>
+  <si>
+    <t>(Id-FirstName-LastName-Club-BirtCity)</t>
   </si>
 </sst>
 </file>
@@ -469,17 +472,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -527,6 +530,9 @@
       <c r="B6" t="s">
         <v>6</v>
       </c>
+      <c r="C6" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B7" t="s">

</xml_diff>

<commit_message>
Entry for Relational Tables and made some properations
</commit_message>
<xml_diff>
--- a/SqlLessons.xlsx
+++ b/SqlLessons.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hasan\Desktop\MSSql\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91B26E51-3879-47E4-86BA-876D3EDA7F7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB810FA5-122B-4826-A801-A05607ED2718}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="74">
   <si>
     <t>cutomer</t>
   </si>
@@ -139,6 +140,114 @@
   </si>
   <si>
     <t>(Id-Title)</t>
+  </si>
+  <si>
+    <t>James</t>
+  </si>
+  <si>
+    <t>Hughes</t>
+  </si>
+  <si>
+    <t>Chess</t>
+  </si>
+  <si>
+    <t>Manchester</t>
+  </si>
+  <si>
+    <t>Michael</t>
+  </si>
+  <si>
+    <t>Moore</t>
+  </si>
+  <si>
+    <t>Math</t>
+  </si>
+  <si>
+    <t>Boby</t>
+  </si>
+  <si>
+    <t>Smith</t>
+  </si>
+  <si>
+    <t>Tennis</t>
+  </si>
+  <si>
+    <t>Birmingham</t>
+  </si>
+  <si>
+    <t>Amanda</t>
+  </si>
+  <si>
+    <t>Brown</t>
+  </si>
+  <si>
+    <t>Music</t>
+  </si>
+  <si>
+    <t>Bristol</t>
+  </si>
+  <si>
+    <t>Jennifer</t>
+  </si>
+  <si>
+    <t>Circle</t>
+  </si>
+  <si>
+    <t>London</t>
+  </si>
+  <si>
+    <t>Benedict</t>
+  </si>
+  <si>
+    <t>Caitlyn</t>
+  </si>
+  <si>
+    <t>Shooter</t>
+  </si>
+  <si>
+    <t>Edinburgh</t>
+  </si>
+  <si>
+    <t>Zilean</t>
+  </si>
+  <si>
+    <t>Bomber</t>
+  </si>
+  <si>
+    <t>Liverpool</t>
+  </si>
+  <si>
+    <t>Biology</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>FIRSTNAME</t>
+  </si>
+  <si>
+    <t>LASTNAME</t>
+  </si>
+  <si>
+    <t>CLUB</t>
+  </si>
+  <si>
+    <t>BIRTHCITY</t>
+  </si>
+  <si>
+    <t>LESSONS</t>
+  </si>
+  <si>
+    <t>EXAMONE</t>
+  </si>
+  <si>
+    <t>EXAMTWO</t>
+  </si>
+  <si>
+    <t>EXAMTHREE</t>
+  </si>
+  <si>
+    <t>STUDENID</t>
   </si>
 </sst>
 </file>
@@ -185,13 +294,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -475,7 +588,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
@@ -682,4 +795,537 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95E4B282-85E4-4FE6-877D-B481A457561E}">
+  <dimension ref="A1:W17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="S5" sqref="S5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="4" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" style="4" customWidth="1"/>
+    <col min="3" max="3" width="10.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.140625" style="4" customWidth="1"/>
+    <col min="6" max="7" width="9.140625" style="4"/>
+    <col min="8" max="8" width="3.28515625" style="4" customWidth="1"/>
+    <col min="9" max="9" width="9.140625" style="4"/>
+    <col min="10" max="10" width="8" style="4" customWidth="1"/>
+    <col min="11" max="11" width="4.140625" style="4" customWidth="1"/>
+    <col min="12" max="12" width="11.7109375" style="4" customWidth="1"/>
+    <col min="13" max="13" width="9.140625" style="4" customWidth="1"/>
+    <col min="14" max="14" width="10" style="4" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="22" max="16384" width="9.140625" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="O1" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="P1" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A2" s="5">
+        <v>25</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="H2" s="5">
+        <v>1</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="K2" s="5">
+        <v>1</v>
+      </c>
+      <c r="L2" s="5">
+        <v>25</v>
+      </c>
+      <c r="M2" s="5">
+        <v>1</v>
+      </c>
+      <c r="N2" s="5">
+        <v>55</v>
+      </c>
+      <c r="O2" s="5">
+        <v>45</v>
+      </c>
+      <c r="P2" s="5">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A3" s="5">
+        <v>35</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="H3" s="5">
+        <v>2</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="K3" s="5">
+        <v>2</v>
+      </c>
+      <c r="L3" s="5">
+        <v>25</v>
+      </c>
+      <c r="M3" s="5">
+        <v>2</v>
+      </c>
+      <c r="N3" s="5">
+        <v>75</v>
+      </c>
+      <c r="O3" s="5">
+        <v>35</v>
+      </c>
+      <c r="P3" s="5">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A4" s="5">
+        <v>67</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
+      <c r="K4" s="5">
+        <v>3</v>
+      </c>
+      <c r="L4" s="5">
+        <v>35</v>
+      </c>
+      <c r="M4" s="5">
+        <v>1</v>
+      </c>
+      <c r="N4" s="5">
+        <v>95</v>
+      </c>
+      <c r="O4" s="5">
+        <v>75</v>
+      </c>
+      <c r="P4" s="5">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A5" s="5">
+        <v>77</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="K5" s="5">
+        <v>5</v>
+      </c>
+      <c r="L5" s="5">
+        <v>35</v>
+      </c>
+      <c r="M5" s="5">
+        <v>2</v>
+      </c>
+      <c r="N5" s="5">
+        <v>25</v>
+      </c>
+      <c r="O5" s="5">
+        <v>65</v>
+      </c>
+      <c r="P5" s="5">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A6" s="5">
+        <v>87</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="K6" s="5">
+        <v>6</v>
+      </c>
+      <c r="L6" s="5">
+        <v>67</v>
+      </c>
+      <c r="M6" s="5">
+        <v>1</v>
+      </c>
+      <c r="N6" s="5">
+        <v>45</v>
+      </c>
+      <c r="O6" s="5">
+        <v>89</v>
+      </c>
+      <c r="P6" s="5">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A7" s="5">
+        <v>97</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="K7" s="5">
+        <v>7</v>
+      </c>
+      <c r="L7" s="5">
+        <v>67</v>
+      </c>
+      <c r="M7" s="5">
+        <v>2</v>
+      </c>
+      <c r="N7" s="5">
+        <v>45</v>
+      </c>
+      <c r="O7" s="5">
+        <v>87</v>
+      </c>
+      <c r="P7" s="5">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A8" s="5">
+        <v>107</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="K8" s="5">
+        <v>8</v>
+      </c>
+      <c r="L8" s="5">
+        <v>77</v>
+      </c>
+      <c r="M8" s="5">
+        <v>1</v>
+      </c>
+      <c r="N8" s="5">
+        <v>25</v>
+      </c>
+      <c r="O8" s="5">
+        <v>36</v>
+      </c>
+      <c r="P8" s="5">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A9" s="5">
+        <v>117</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="K9" s="5">
+        <v>9</v>
+      </c>
+      <c r="L9" s="5">
+        <v>77</v>
+      </c>
+      <c r="M9" s="5">
+        <v>2</v>
+      </c>
+      <c r="N9" s="5">
+        <v>75</v>
+      </c>
+      <c r="O9" s="5">
+        <v>85</v>
+      </c>
+      <c r="P9" s="5">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A10" s="5"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="K10" s="5">
+        <v>10</v>
+      </c>
+      <c r="L10" s="5">
+        <v>87</v>
+      </c>
+      <c r="M10" s="5">
+        <v>1</v>
+      </c>
+      <c r="N10" s="5">
+        <v>45</v>
+      </c>
+      <c r="O10" s="5">
+        <v>98</v>
+      </c>
+      <c r="P10" s="5">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="K11" s="5">
+        <v>11</v>
+      </c>
+      <c r="L11" s="5">
+        <v>87</v>
+      </c>
+      <c r="M11" s="5">
+        <v>2</v>
+      </c>
+      <c r="N11" s="5">
+        <v>12</v>
+      </c>
+      <c r="O11" s="5">
+        <v>25</v>
+      </c>
+      <c r="P11" s="5">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="K12" s="5">
+        <v>12</v>
+      </c>
+      <c r="L12" s="5">
+        <v>97</v>
+      </c>
+      <c r="M12" s="5">
+        <v>1</v>
+      </c>
+      <c r="N12" s="5">
+        <v>45</v>
+      </c>
+      <c r="O12" s="5">
+        <v>68</v>
+      </c>
+      <c r="P12" s="5">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="K13" s="5">
+        <v>13</v>
+      </c>
+      <c r="L13" s="5">
+        <v>97</v>
+      </c>
+      <c r="M13" s="5">
+        <v>2</v>
+      </c>
+      <c r="N13" s="5">
+        <v>98</v>
+      </c>
+      <c r="O13" s="5">
+        <v>45</v>
+      </c>
+      <c r="P13" s="5">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="K14" s="5">
+        <v>14</v>
+      </c>
+      <c r="L14" s="5">
+        <v>107</v>
+      </c>
+      <c r="M14" s="5">
+        <v>1</v>
+      </c>
+      <c r="N14" s="5">
+        <v>45</v>
+      </c>
+      <c r="O14" s="5">
+        <v>87</v>
+      </c>
+      <c r="P14" s="5">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="K15" s="5">
+        <v>15</v>
+      </c>
+      <c r="L15" s="5">
+        <v>107</v>
+      </c>
+      <c r="M15" s="5">
+        <v>2</v>
+      </c>
+      <c r="N15" s="5">
+        <v>75</v>
+      </c>
+      <c r="O15" s="5">
+        <v>85</v>
+      </c>
+      <c r="P15" s="5">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="K16" s="5">
+        <v>16</v>
+      </c>
+      <c r="L16" s="5">
+        <v>117</v>
+      </c>
+      <c r="M16" s="5">
+        <v>1</v>
+      </c>
+      <c r="N16" s="5">
+        <v>75</v>
+      </c>
+      <c r="O16" s="5">
+        <v>65</v>
+      </c>
+      <c r="P16" s="5">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="17" spans="11:16" x14ac:dyDescent="0.25">
+      <c r="K17" s="5">
+        <v>17</v>
+      </c>
+      <c r="L17" s="5">
+        <v>117</v>
+      </c>
+      <c r="M17" s="5">
+        <v>2</v>
+      </c>
+      <c r="N17" s="5">
+        <v>35</v>
+      </c>
+      <c r="O17" s="5">
+        <v>85</v>
+      </c>
+      <c r="P17" s="5">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
One to One and One to Many Relations
</commit_message>
<xml_diff>
--- a/SqlLessons.xlsx
+++ b/SqlLessons.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hasan\Desktop\MSSql\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB810FA5-122B-4826-A801-A05607ED2718}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04B544A3-843D-47E3-B0E3-F10667469F87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="95">
   <si>
     <t>cutomer</t>
   </si>
@@ -248,6 +249,69 @@
   </si>
   <si>
     <t>STUDENID</t>
+  </si>
+  <si>
+    <t>product</t>
+  </si>
+  <si>
+    <t>fridge</t>
+  </si>
+  <si>
+    <t>tv</t>
+  </si>
+  <si>
+    <t>laptop</t>
+  </si>
+  <si>
+    <t>foodsaver</t>
+  </si>
+  <si>
+    <t>multibox</t>
+  </si>
+  <si>
+    <t>tea glass</t>
+  </si>
+  <si>
+    <t>category</t>
+  </si>
+  <si>
+    <t>electronics</t>
+  </si>
+  <si>
+    <t>household</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>price</t>
+  </si>
+  <si>
+    <t>stock</t>
+  </si>
+  <si>
+    <t>colour</t>
+  </si>
+  <si>
+    <t>height</t>
+  </si>
+  <si>
+    <t>weight</t>
+  </si>
+  <si>
+    <t>red</t>
+  </si>
+  <si>
+    <t>specificationId</t>
+  </si>
+  <si>
+    <t>laptopm</t>
+  </si>
+  <si>
+    <t>..</t>
   </si>
 </sst>
 </file>
@@ -294,15 +358,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -799,530 +862,663 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95E4B282-85E4-4FE6-877D-B481A457561E}">
-  <dimension ref="A1:W17"/>
+  <dimension ref="A1:P17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="S5" sqref="S5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125" style="4" customWidth="1"/>
-    <col min="3" max="3" width="10.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.140625" style="4" customWidth="1"/>
-    <col min="6" max="7" width="9.140625" style="4"/>
-    <col min="8" max="8" width="3.28515625" style="4" customWidth="1"/>
-    <col min="9" max="9" width="9.140625" style="4"/>
-    <col min="10" max="10" width="8" style="4" customWidth="1"/>
-    <col min="11" max="11" width="4.140625" style="4" customWidth="1"/>
-    <col min="12" max="12" width="11.7109375" style="4" customWidth="1"/>
-    <col min="13" max="13" width="9.140625" style="4" customWidth="1"/>
-    <col min="14" max="14" width="10" style="4" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.42578125" style="4" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="22" max="16384" width="9.140625" style="4"/>
+    <col min="1" max="1" width="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" customWidth="1"/>
+    <col min="3" max="3" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.140625" customWidth="1"/>
+    <col min="8" max="8" width="3.28515625" customWidth="1"/>
+    <col min="10" max="10" width="8" customWidth="1"/>
+    <col min="11" max="11" width="4.140625" customWidth="1"/>
+    <col min="12" max="12" width="11.7109375" customWidth="1"/>
+    <col min="13" max="13" width="9.140625" customWidth="1"/>
+    <col min="14" max="14" width="10" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" t="s">
         <v>64</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" t="s">
         <v>65</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" t="s">
         <v>66</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" t="s">
         <v>67</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" t="s">
         <v>68</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" t="s">
         <v>64</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" t="s">
         <v>69</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="K1" t="s">
         <v>64</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="L1" t="s">
         <v>73</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="M1" t="s">
         <v>69</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="N1" t="s">
         <v>70</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="O1" t="s">
         <v>71</v>
       </c>
-      <c r="P1" s="4" t="s">
+      <c r="P1" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A2" s="5">
+      <c r="A2" s="4">
         <v>25</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="H2" s="5">
+      <c r="H2" s="4">
         <v>1</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="I2" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="K2" s="5">
+      <c r="K2" s="4">
         <v>1</v>
       </c>
-      <c r="L2" s="5">
+      <c r="L2" s="4">
         <v>25</v>
       </c>
-      <c r="M2" s="5">
+      <c r="M2" s="4">
         <v>1</v>
       </c>
-      <c r="N2" s="5">
+      <c r="N2" s="4">
         <v>55</v>
       </c>
-      <c r="O2" s="5">
+      <c r="O2" s="4">
         <v>45</v>
       </c>
-      <c r="P2" s="5">
+      <c r="P2" s="4">
         <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A3" s="5">
+      <c r="A3" s="4">
         <v>35</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="H3" s="5">
+      <c r="H3" s="4">
         <v>2</v>
       </c>
-      <c r="I3" s="5" t="s">
+      <c r="I3" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="K3" s="5">
+      <c r="K3" s="4">
         <v>2</v>
       </c>
-      <c r="L3" s="5">
+      <c r="L3" s="4">
         <v>25</v>
       </c>
-      <c r="M3" s="5">
+      <c r="M3" s="4">
         <v>2</v>
       </c>
-      <c r="N3" s="5">
+      <c r="N3" s="4">
         <v>75</v>
       </c>
-      <c r="O3" s="5">
+      <c r="O3" s="4">
         <v>35</v>
       </c>
-      <c r="P3" s="5">
+      <c r="P3" s="4">
         <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A4" s="5">
+      <c r="A4" s="4">
         <v>67</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E4" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="H4" s="5"/>
-      <c r="I4" s="5"/>
-      <c r="K4" s="5">
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+      <c r="K4" s="4">
         <v>3</v>
       </c>
-      <c r="L4" s="5">
+      <c r="L4" s="4">
         <v>35</v>
       </c>
-      <c r="M4" s="5">
+      <c r="M4" s="4">
         <v>1</v>
       </c>
-      <c r="N4" s="5">
+      <c r="N4" s="4">
         <v>95</v>
       </c>
-      <c r="O4" s="5">
+      <c r="O4" s="4">
         <v>75</v>
       </c>
-      <c r="P4" s="5">
+      <c r="P4" s="4">
         <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A5" s="5">
+      <c r="A5" s="4">
         <v>77</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="E5" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="K5" s="5">
+      <c r="K5" s="4">
         <v>5</v>
       </c>
-      <c r="L5" s="5">
+      <c r="L5" s="4">
         <v>35</v>
       </c>
-      <c r="M5" s="5">
+      <c r="M5" s="4">
         <v>2</v>
       </c>
-      <c r="N5" s="5">
+      <c r="N5" s="4">
         <v>25</v>
       </c>
-      <c r="O5" s="5">
+      <c r="O5" s="4">
         <v>65</v>
       </c>
-      <c r="P5" s="5">
+      <c r="P5" s="4">
         <v>98</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A6" s="5">
+      <c r="A6" s="4">
         <v>87</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D6" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="E6" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="K6" s="5">
+      <c r="K6" s="4">
         <v>6</v>
       </c>
-      <c r="L6" s="5">
+      <c r="L6" s="4">
         <v>67</v>
       </c>
-      <c r="M6" s="5">
+      <c r="M6" s="4">
         <v>1</v>
       </c>
-      <c r="N6" s="5">
+      <c r="N6" s="4">
         <v>45</v>
       </c>
-      <c r="O6" s="5">
+      <c r="O6" s="4">
         <v>89</v>
       </c>
-      <c r="P6" s="5">
+      <c r="P6" s="4">
         <v>78</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A7" s="5">
+      <c r="A7" s="4">
         <v>97</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="D7" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="E7" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="K7" s="5">
+      <c r="K7" s="4">
         <v>7</v>
       </c>
-      <c r="L7" s="5">
+      <c r="L7" s="4">
         <v>67</v>
       </c>
-      <c r="M7" s="5">
+      <c r="M7" s="4">
         <v>2</v>
       </c>
-      <c r="N7" s="5">
+      <c r="N7" s="4">
         <v>45</v>
       </c>
-      <c r="O7" s="5">
+      <c r="O7" s="4">
         <v>87</v>
       </c>
-      <c r="P7" s="5">
+      <c r="P7" s="4">
         <v>89</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A8" s="5">
+      <c r="A8" s="4">
         <v>107</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="D8" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="E8" s="5" t="s">
+      <c r="E8" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="K8" s="5">
+      <c r="K8" s="4">
         <v>8</v>
       </c>
-      <c r="L8" s="5">
+      <c r="L8" s="4">
         <v>77</v>
       </c>
-      <c r="M8" s="5">
+      <c r="M8" s="4">
         <v>1</v>
       </c>
-      <c r="N8" s="5">
+      <c r="N8" s="4">
         <v>25</v>
       </c>
-      <c r="O8" s="5">
+      <c r="O8" s="4">
         <v>36</v>
       </c>
-      <c r="P8" s="5">
+      <c r="P8" s="4">
         <v>64</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A9" s="5">
+      <c r="A9" s="4">
         <v>117</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C9" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="D9" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="E9" s="5" t="s">
+      <c r="E9" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="K9" s="5">
+      <c r="K9" s="4">
         <v>9</v>
       </c>
-      <c r="L9" s="5">
+      <c r="L9" s="4">
         <v>77</v>
       </c>
-      <c r="M9" s="5">
+      <c r="M9" s="4">
         <v>2</v>
       </c>
-      <c r="N9" s="5">
+      <c r="N9" s="4">
         <v>75</v>
       </c>
-      <c r="O9" s="5">
+      <c r="O9" s="4">
         <v>85</v>
       </c>
-      <c r="P9" s="5">
+      <c r="P9" s="4">
         <v>85</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A10" s="5"/>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="K10" s="5">
+      <c r="A10" s="4"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="K10" s="4">
         <v>10</v>
       </c>
-      <c r="L10" s="5">
+      <c r="L10" s="4">
         <v>87</v>
       </c>
-      <c r="M10" s="5">
+      <c r="M10" s="4">
         <v>1</v>
       </c>
-      <c r="N10" s="5">
+      <c r="N10" s="4">
         <v>45</v>
       </c>
-      <c r="O10" s="5">
+      <c r="O10" s="4">
         <v>98</v>
       </c>
-      <c r="P10" s="5">
+      <c r="P10" s="4">
         <v>85</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="K11" s="5">
+      <c r="K11" s="4">
         <v>11</v>
       </c>
-      <c r="L11" s="5">
+      <c r="L11" s="4">
         <v>87</v>
       </c>
-      <c r="M11" s="5">
+      <c r="M11" s="4">
         <v>2</v>
       </c>
-      <c r="N11" s="5">
+      <c r="N11" s="4">
         <v>12</v>
       </c>
-      <c r="O11" s="5">
+      <c r="O11" s="4">
         <v>25</v>
       </c>
-      <c r="P11" s="5">
+      <c r="P11" s="4">
         <v>75</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="K12" s="5">
+      <c r="K12" s="4">
         <v>12</v>
       </c>
-      <c r="L12" s="5">
+      <c r="L12" s="4">
         <v>97</v>
       </c>
-      <c r="M12" s="5">
+      <c r="M12" s="4">
         <v>1</v>
       </c>
-      <c r="N12" s="5">
+      <c r="N12" s="4">
         <v>45</v>
       </c>
-      <c r="O12" s="5">
+      <c r="O12" s="4">
         <v>68</v>
       </c>
-      <c r="P12" s="5">
+      <c r="P12" s="4">
         <v>96</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="K13" s="5">
+      <c r="K13" s="4">
         <v>13</v>
       </c>
-      <c r="L13" s="5">
+      <c r="L13" s="4">
         <v>97</v>
       </c>
-      <c r="M13" s="5">
+      <c r="M13" s="4">
         <v>2</v>
       </c>
-      <c r="N13" s="5">
+      <c r="N13" s="4">
         <v>98</v>
       </c>
-      <c r="O13" s="5">
+      <c r="O13" s="4">
         <v>45</v>
       </c>
-      <c r="P13" s="5">
+      <c r="P13" s="4">
         <v>75</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="K14" s="5">
+      <c r="K14" s="4">
         <v>14</v>
       </c>
-      <c r="L14" s="5">
+      <c r="L14" s="4">
         <v>107</v>
       </c>
-      <c r="M14" s="5">
+      <c r="M14" s="4">
         <v>1</v>
       </c>
-      <c r="N14" s="5">
+      <c r="N14" s="4">
         <v>45</v>
       </c>
-      <c r="O14" s="5">
+      <c r="O14" s="4">
         <v>87</v>
       </c>
-      <c r="P14" s="5">
+      <c r="P14" s="4">
         <v>85</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="K15" s="5">
+      <c r="K15" s="4">
         <v>15</v>
       </c>
-      <c r="L15" s="5">
+      <c r="L15" s="4">
         <v>107</v>
       </c>
-      <c r="M15" s="5">
+      <c r="M15" s="4">
         <v>2</v>
       </c>
-      <c r="N15" s="5">
+      <c r="N15" s="4">
         <v>75</v>
       </c>
-      <c r="O15" s="5">
+      <c r="O15" s="4">
         <v>85</v>
       </c>
-      <c r="P15" s="5">
+      <c r="P15" s="4">
         <v>86</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="K16" s="5">
+      <c r="K16" s="4">
         <v>16</v>
       </c>
-      <c r="L16" s="5">
+      <c r="L16" s="4">
         <v>117</v>
       </c>
-      <c r="M16" s="5">
+      <c r="M16" s="4">
         <v>1</v>
       </c>
-      <c r="N16" s="5">
+      <c r="N16" s="4">
         <v>75</v>
       </c>
-      <c r="O16" s="5">
+      <c r="O16" s="4">
         <v>65</v>
       </c>
-      <c r="P16" s="5">
+      <c r="P16" s="4">
         <v>65</v>
       </c>
     </row>
     <row r="17" spans="11:16" x14ac:dyDescent="0.25">
-      <c r="K17" s="5">
+      <c r="K17" s="4">
         <v>17</v>
       </c>
-      <c r="L17" s="5">
+      <c r="L17" s="4">
         <v>117</v>
       </c>
-      <c r="M17" s="5">
+      <c r="M17" s="4">
         <v>2</v>
       </c>
-      <c r="N17" s="5">
+      <c r="N17" s="4">
         <v>35</v>
       </c>
-      <c r="O17" s="5">
+      <c r="O17" s="4">
         <v>85</v>
       </c>
-      <c r="P17" s="5">
+      <c r="P17" s="4">
         <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A11DB34-C4C1-4660-B249-DE136EACB83D}">
+  <dimension ref="A1:P10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="K5" sqref="K5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="11" max="11" width="14.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C1" t="s">
+        <v>81</v>
+      </c>
+      <c r="G1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="G2" t="s">
+        <v>84</v>
+      </c>
+      <c r="H2" t="s">
+        <v>85</v>
+      </c>
+      <c r="I2" t="s">
+        <v>86</v>
+      </c>
+      <c r="J2" t="s">
+        <v>87</v>
+      </c>
+      <c r="K2" t="s">
+        <v>92</v>
+      </c>
+      <c r="M2" t="s">
+        <v>84</v>
+      </c>
+      <c r="N2" t="s">
+        <v>88</v>
+      </c>
+      <c r="O2" t="s">
+        <v>89</v>
+      </c>
+      <c r="P2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>75</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3" t="s">
+        <v>75</v>
+      </c>
+      <c r="I3">
+        <v>250</v>
+      </c>
+      <c r="J3">
+        <v>15</v>
+      </c>
+      <c r="K3">
+        <v>1</v>
+      </c>
+      <c r="M3">
+        <v>1</v>
+      </c>
+      <c r="N3" t="s">
+        <v>91</v>
+      </c>
+      <c r="O3">
+        <v>95</v>
+      </c>
+      <c r="P3">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C4" t="s">
+        <v>82</v>
+      </c>
+      <c r="G4">
+        <v>2</v>
+      </c>
+      <c r="H4" t="s">
+        <v>93</v>
+      </c>
+      <c r="I4">
+        <v>125</v>
+      </c>
+      <c r="J4">
+        <v>12</v>
+      </c>
+      <c r="K4" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>79</v>
+      </c>
+      <c r="C9" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>80</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Many to Many Lessons
</commit_message>
<xml_diff>
--- a/SqlLessons.xlsx
+++ b/SqlLessons.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hasan\Desktop\MSSql\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04B544A3-843D-47E3-B0E3-F10667469F87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{393660DB-A19F-4308-8F16-7918D4991CC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="109">
   <si>
     <t>cutomer</t>
   </si>
@@ -312,6 +312,48 @@
   </si>
   <si>
     <t>..</t>
+  </si>
+  <si>
+    <t>MANY TO MANY</t>
+  </si>
+  <si>
+    <t>USERS</t>
+  </si>
+  <si>
+    <t>CLAIMS</t>
+  </si>
+  <si>
+    <t>USERCLAIMS</t>
+  </si>
+  <si>
+    <t>NAME</t>
+  </si>
+  <si>
+    <t>MICHAEL</t>
+  </si>
+  <si>
+    <t>GABRIEL</t>
+  </si>
+  <si>
+    <t>AMANDA</t>
+  </si>
+  <si>
+    <t>TITLE</t>
+  </si>
+  <si>
+    <t>ACCOUNT ACC</t>
+  </si>
+  <si>
+    <t>SALES ACC</t>
+  </si>
+  <si>
+    <t>PURCHASE ACC</t>
+  </si>
+  <si>
+    <t>USERID</t>
+  </si>
+  <si>
+    <t>CLAIMSID</t>
   </si>
 </sst>
 </file>
@@ -358,7 +400,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -367,6 +409,9 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1392,10 +1437,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A11DB34-C4C1-4660-B249-DE136EACB83D}">
-  <dimension ref="A1:P10"/>
+  <dimension ref="A1:P20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+      <selection activeCell="P15" sqref="P15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1520,6 +1565,156 @@
       <c r="A10" t="s">
         <v>80</v>
       </c>
+      <c r="G10" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="G12" t="s">
+        <v>96</v>
+      </c>
+      <c r="J12" t="s">
+        <v>97</v>
+      </c>
+      <c r="M12" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="F13" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="G13" t="s">
+        <v>99</v>
+      </c>
+      <c r="I13" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="J13" t="s">
+        <v>103</v>
+      </c>
+      <c r="L13" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="M13" t="s">
+        <v>107</v>
+      </c>
+      <c r="N13" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="F14">
+        <v>1</v>
+      </c>
+      <c r="G14" t="s">
+        <v>100</v>
+      </c>
+      <c r="I14">
+        <v>1</v>
+      </c>
+      <c r="J14" t="s">
+        <v>104</v>
+      </c>
+      <c r="L14">
+        <v>1</v>
+      </c>
+      <c r="M14">
+        <v>1</v>
+      </c>
+      <c r="N14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="F15">
+        <v>2</v>
+      </c>
+      <c r="G15" t="s">
+        <v>101</v>
+      </c>
+      <c r="I15">
+        <v>2</v>
+      </c>
+      <c r="J15" t="s">
+        <v>105</v>
+      </c>
+      <c r="L15">
+        <v>2</v>
+      </c>
+      <c r="M15">
+        <v>1</v>
+      </c>
+      <c r="N15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="F16">
+        <v>3</v>
+      </c>
+      <c r="G16" t="s">
+        <v>102</v>
+      </c>
+      <c r="I16">
+        <v>3</v>
+      </c>
+      <c r="J16" t="s">
+        <v>106</v>
+      </c>
+      <c r="L16">
+        <v>3</v>
+      </c>
+      <c r="M16">
+        <v>2</v>
+      </c>
+      <c r="N16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="12:14" x14ac:dyDescent="0.25">
+      <c r="L17">
+        <v>4</v>
+      </c>
+      <c r="M17">
+        <v>2</v>
+      </c>
+      <c r="N17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="12:14" x14ac:dyDescent="0.25">
+      <c r="L18">
+        <v>5</v>
+      </c>
+      <c r="M18">
+        <v>2</v>
+      </c>
+      <c r="N18">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="12:14" x14ac:dyDescent="0.25">
+      <c r="L19">
+        <v>6</v>
+      </c>
+      <c r="M19">
+        <v>3</v>
+      </c>
+      <c r="N19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="12:14" x14ac:dyDescent="0.25">
+      <c r="L20">
+        <v>7</v>
+      </c>
+      <c r="M20">
+        <v>3</v>
+      </c>
+      <c r="N20">
+        <v>3</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
New table and DDL commands Practise
</commit_message>
<xml_diff>
--- a/SqlLessons.xlsx
+++ b/SqlLessons.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hasan\Desktop\MSSql\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{393660DB-A19F-4308-8F16-7918D4991CC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4A45C9C-2101-4D5C-8A85-0665BC457A62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="132">
   <si>
     <t>cutomer</t>
   </si>
@@ -354,6 +355,75 @@
   </si>
   <si>
     <t>CLAIMSID</t>
+  </si>
+  <si>
+    <t>DBACCOUNT</t>
+  </si>
+  <si>
+    <t>TBLPRODUCTS</t>
+  </si>
+  <si>
+    <t>TBLCLIENTS</t>
+  </si>
+  <si>
+    <t>TBLEMPLOYEE</t>
+  </si>
+  <si>
+    <t>TBLSALES</t>
+  </si>
+  <si>
+    <t>TBLCATEGORIES</t>
+  </si>
+  <si>
+    <t>TBLCITIES</t>
+  </si>
+  <si>
+    <t>BRAND</t>
+  </si>
+  <si>
+    <t>CATEGORYID</t>
+  </si>
+  <si>
+    <t>COSTPRICE</t>
+  </si>
+  <si>
+    <t>SELLPRICE</t>
+  </si>
+  <si>
+    <t>STOCKLEVEL</t>
+  </si>
+  <si>
+    <t>STATUS</t>
+  </si>
+  <si>
+    <t>FULLNAME</t>
+  </si>
+  <si>
+    <t>CITYID</t>
+  </si>
+  <si>
+    <t>BALANCE</t>
+  </si>
+  <si>
+    <t>PRODUCTID</t>
+  </si>
+  <si>
+    <t>CLIENTID</t>
+  </si>
+  <si>
+    <t>EMPLOYEEID</t>
+  </si>
+  <si>
+    <t>QUANTITY</t>
+  </si>
+  <si>
+    <t>TOTAL</t>
+  </si>
+  <si>
+    <t>DATE</t>
+  </si>
+  <si>
+    <t>LOCATION</t>
   </si>
 </sst>
 </file>
@@ -1439,7 +1509,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A11DB34-C4C1-4660-B249-DE136EACB83D}">
   <dimension ref="A1:P20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="P15" sqref="P15"/>
     </sheetView>
   </sheetViews>
@@ -1719,4 +1789,138 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{233AFF21-8B60-491D-B43D-157D450DC524}">
+  <dimension ref="A1:Q12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K14" sqref="K14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>111</v>
+      </c>
+      <c r="D3" t="s">
+        <v>110</v>
+      </c>
+      <c r="G3" t="s">
+        <v>112</v>
+      </c>
+      <c r="J3" t="s">
+        <v>113</v>
+      </c>
+      <c r="M3" t="s">
+        <v>114</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>64</v>
+      </c>
+      <c r="D5" t="s">
+        <v>64</v>
+      </c>
+      <c r="G5" t="s">
+        <v>64</v>
+      </c>
+      <c r="J5" t="s">
+        <v>64</v>
+      </c>
+      <c r="M5" t="s">
+        <v>64</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>65</v>
+      </c>
+      <c r="D6" t="s">
+        <v>99</v>
+      </c>
+      <c r="G6" t="s">
+        <v>122</v>
+      </c>
+      <c r="J6" t="s">
+        <v>125</v>
+      </c>
+      <c r="M6" t="s">
+        <v>103</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>66</v>
+      </c>
+      <c r="D7" t="s">
+        <v>116</v>
+      </c>
+      <c r="J7" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>123</v>
+      </c>
+      <c r="D8" t="s">
+        <v>117</v>
+      </c>
+      <c r="J8" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>124</v>
+      </c>
+      <c r="D9" t="s">
+        <v>118</v>
+      </c>
+      <c r="J9" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="D10" t="s">
+        <v>119</v>
+      </c>
+      <c r="J10" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="D11" t="s">
+        <v>120</v>
+      </c>
+      <c r="J11" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="D12" t="s">
+        <v>121</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>